<commit_message>
El Verde rainfall data wrangling and figures
</commit_message>
<xml_diff>
--- a/ArrayGHG-Data-Raw/Soil-data-LeileiWhendee/070715_pH_PuertoRico 2015 drought.xlsx
+++ b/ArrayGHG-Data-Raw/Soil-data-LeileiWhendee/070715_pH_PuertoRico 2015 drought.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christine/Documents/GITHUB/cso040code_ArrayGHG/ArrayGHG-Data-Raw/Soil-data-LeileiWhendee/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="400" windowWidth="25420" windowHeight="15220"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="25420" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -328,20 +333,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2138426440"/>
-        <c:axId val="-2137776168"/>
+        <c:axId val="-2023387632"/>
+        <c:axId val="-2022049040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2138426440"/>
+        <c:axId val="-2023387632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137776168"/>
+        <c:crossAx val="-2022049040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -349,7 +355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137776168"/>
+        <c:axId val="-2022049040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.4"/>
@@ -362,7 +368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138426440"/>
+        <c:crossAx val="-2023387632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -507,20 +513,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2139178488"/>
-        <c:axId val="-2139187736"/>
+        <c:axId val="-2059640432"/>
+        <c:axId val="-2112551696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2139178488"/>
+        <c:axId val="-2059640432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139187736"/>
+        <c:crossAx val="-2112551696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -528,7 +535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2139187736"/>
+        <c:axId val="-2112551696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.0"/>
@@ -540,7 +547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139178488"/>
+        <c:crossAx val="-2059640432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -916,11 +923,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="7" customWidth="1"/>
@@ -928,7 +935,7 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26">
+    <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -997,7 +1004,7 @@
         <v>5.4797607409245386E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1037,7 +1044,7 @@
         <v>7.7132641886846112E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1077,7 +1084,7 @@
         <v>7.633260552782592E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1117,7 +1124,7 @@
         <v>7.2422372233999624E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1146,7 +1153,7 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1175,7 +1182,7 @@
         <v>4.49</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1204,7 +1211,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1262,7 +1269,7 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1291,7 +1298,7 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1320,7 +1327,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1349,7 +1356,7 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1378,7 +1385,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1465,7 +1472,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1523,7 +1530,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1552,7 +1559,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1581,7 +1588,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1639,7 +1646,7 @@
         <v>5.27</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1668,7 +1675,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1697,7 +1704,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1731,7 +1738,7 @@
         <v>7.649255591958673E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>9.5524865872713999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1799,7 +1806,7 @@
         <v>0.10078855755160565</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1833,7 +1840,7 @@
         <v>9.4891751192843099E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1856,7 +1863,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1879,7 +1886,7 @@
         <v>4.6100000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1902,7 +1909,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1925,7 +1932,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1948,7 +1955,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1971,7 +1978,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1994,7 +2001,7 @@
         <v>5.01</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2017,7 +2024,7 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2040,7 +2047,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2063,7 +2070,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2086,7 +2093,7 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2109,7 +2116,7 @@
         <v>5.27</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2132,7 +2139,7 @@
         <v>4.93</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2155,7 +2162,7 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2178,7 +2185,7 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>5.32</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2224,7 +2231,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2247,7 +2254,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2270,7 +2277,7 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2297,11 +2304,6 @@
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2311,14 +2313,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2328,13 +2325,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>